<commit_message>
Add config and pages
</commit_message>
<xml_diff>
--- a/programming-essentials-zb0144/config.xlsx
+++ b/programming-essentials-zb0144/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\canvas-course-scaffolder-with-course-configs\programming-essentials-zb0144\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F49DE07-D85C-4566-B80A-073720F24E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B663288-2B9F-4A7C-877D-5C4B84D0A111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="1140" windowWidth="28800" windowHeight="19305" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47445" yWindow="420" windowWidth="28800" windowHeight="19305" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemene info" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="204">
   <si>
     <t>Naam</t>
   </si>
@@ -558,9 +558,6 @@
     <t>11 - Debugging</t>
   </si>
   <si>
-    <t>Algemene informatie</t>
-  </si>
-  <si>
     <t>https://thomasmore365-my.sharepoint.com/:p:/g/personal/u0134243_thomasmore_be/ERTv-9Iw_4REkHhNtgWr-EMBZ0AsPc3Uyl891mxnDyfBQQ?e=S2XGUa</t>
   </si>
   <si>
@@ -640,6 +637,27 @@
   </si>
   <si>
     <t>https://thomasmore365-my.sharepoint.com/:p:/g/personal/u0134243_thomasmore_be/Eba1uodVpnJJuxqZkWgw3cYBd0wCeiUO_NuDqi1j_JOBYQ?e=3N9RZU</t>
+  </si>
+  <si>
+    <t>Algemene informatie (pptx)</t>
+  </si>
+  <si>
+    <t>GitHub classroom assignment</t>
+  </si>
+  <si>
+    <t>https://classroom.github.com/a/SVQ8tyzw</t>
+  </si>
+  <si>
+    <t>Link naar de oefeningen</t>
+  </si>
+  <si>
+    <t>https://it-graduaten-programmingessentials.netlify.app/</t>
+  </si>
+  <si>
+    <t>Link naar CodeGrade</t>
+  </si>
+  <si>
+    <t>https://app.codegra.de/</t>
   </si>
 </sst>
 </file>
@@ -787,8 +805,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:I164" totalsRowShown="0">
-  <autoFilter ref="A1:I164" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:I167" totalsRowShown="0">
+  <autoFilter ref="A1:I167" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F1B940E-7EAD-48A5-AA1E-A5E5ED525C5C}" name="Module"/>
     <tableColumn id="2" xr3:uid="{54A84E46-41BB-4012-84B6-2A4A1FB473F4}" name="Type"/>
@@ -3416,7 +3434,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3553,10 +3571,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E63DFD8-2013-40A2-8CE5-0CB5ABE5CD54}">
-  <dimension ref="A1:I164"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="F137" sqref="F137"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3597,7 +3615,7 @@
         <v>61</v>
       </c>
       <c r="I1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3636,69 +3654,64 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="I5">
-        <v>0</v>
+      <c r="F5" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="I7">
-        <v>0</v>
+      <c r="F7" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3706,16 +3719,17 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C8" t="s">
+        <v>177</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3723,13 +3737,16 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>45</v>
+      <c r="F9" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -3740,16 +3757,17 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
+        <v>176</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3763,7 +3781,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -3780,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -3797,7 +3815,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -3814,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -3831,7 +3849,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -3848,7 +3866,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -3865,7 +3883,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -3882,7 +3900,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -3893,16 +3911,16 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3910,73 +3928,68 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>173</v>
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>172</v>
+      </c>
       <c r="I23">
         <v>0</v>
       </c>
@@ -3986,16 +3999,17 @@
         <v>160</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C24" t="s">
+        <v>177</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
+      <c r="F24" s="2"/>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -4003,13 +4017,16 @@
         <v>160</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
-        <v>50</v>
+      <c r="F25" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -4020,16 +4037,17 @@
         <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C26" t="s">
+        <v>176</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>51</v>
-      </c>
+      <c r="F26" s="2"/>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4043,7 +4061,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -4060,7 +4078,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -4077,7 +4095,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -4094,7 +4112,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -4111,7 +4129,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -4128,7 +4146,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -4145,7 +4163,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -4162,7 +4180,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -4173,16 +4191,16 @@
         <v>160</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
-      </c>
-      <c r="C35" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -4190,73 +4208,68 @@
         <v>160</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>181</v>
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
-      </c>
-      <c r="C37" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
       <c r="I37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>182</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B39" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>180</v>
+      </c>
       <c r="I39">
         <v>0</v>
       </c>
@@ -4266,16 +4279,17 @@
         <v>161</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C40" t="s">
+        <v>177</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40" t="s">
-        <v>72</v>
-      </c>
+      <c r="F40" s="2"/>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4283,13 +4297,16 @@
         <v>161</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="E41" t="s">
-        <v>120</v>
+      <c r="F41" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -4300,16 +4317,17 @@
         <v>161</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C42" t="s">
+        <v>176</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
-      <c r="E42" t="s">
-        <v>121</v>
-      </c>
+      <c r="F42" s="2"/>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4323,7 +4341,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -4340,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -4357,7 +4375,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -4374,7 +4392,7 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -4391,7 +4409,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -4408,7 +4426,7 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -4425,7 +4443,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -4442,7 +4460,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I50">
         <v>1</v>
@@ -4453,16 +4471,16 @@
         <v>161</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>75</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4470,73 +4488,68 @@
         <v>161</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="F52" t="s">
-        <v>183</v>
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>76</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
-      </c>
-      <c r="C53" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="E53" t="s">
+        <v>77</v>
+      </c>
       <c r="I53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>191</v>
+        <v>0</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>182</v>
+      </c>
       <c r="I55">
         <v>0</v>
       </c>
@@ -4546,16 +4559,17 @@
         <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C56" t="s">
+        <v>177</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
-      <c r="E56" t="s">
-        <v>78</v>
-      </c>
+      <c r="F56" s="2"/>
       <c r="I56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4563,13 +4577,16 @@
         <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
-      <c r="E57" t="s">
-        <v>125</v>
+      <c r="F57" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -4580,16 +4597,17 @@
         <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C58" t="s">
+        <v>176</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
-      <c r="E58" t="s">
-        <v>126</v>
-      </c>
+      <c r="F58" s="2"/>
       <c r="I58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -4603,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -4620,7 +4638,7 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I60">
         <v>1</v>
@@ -4637,7 +4655,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -4654,7 +4672,7 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="I62">
         <v>1</v>
@@ -4671,7 +4689,7 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="I63">
         <v>1</v>
@@ -4688,7 +4706,7 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="I64">
         <v>1</v>
@@ -4705,7 +4723,7 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I65">
         <v>1</v>
@@ -4722,7 +4740,7 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I66">
         <v>1</v>
@@ -4733,16 +4751,16 @@
         <v>162</v>
       </c>
       <c r="B67" t="s">
-        <v>175</v>
-      </c>
-      <c r="C67" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>81</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -4750,73 +4768,68 @@
         <v>162</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="F68" t="s">
-        <v>184</v>
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>82</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" t="s">
-        <v>175</v>
-      </c>
-      <c r="C69" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
-      <c r="F69" s="2"/>
+      <c r="E69" t="s">
+        <v>83</v>
+      </c>
       <c r="I69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B70" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C70" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>192</v>
+        <v>0</v>
       </c>
       <c r="I70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="F71" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>183</v>
+      </c>
       <c r="I71">
         <v>0</v>
       </c>
@@ -4826,16 +4839,17 @@
         <v>163</v>
       </c>
       <c r="B72" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C72" t="s">
+        <v>177</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
-      <c r="E72" t="s">
-        <v>84</v>
-      </c>
+      <c r="F72" s="2"/>
       <c r="I72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -4843,13 +4857,16 @@
         <v>163</v>
       </c>
       <c r="B73" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
-      <c r="E73" t="s">
-        <v>130</v>
+      <c r="F73" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="I73">
         <v>1</v>
@@ -4860,16 +4877,17 @@
         <v>163</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C74" t="s">
+        <v>176</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
-      <c r="E74" t="s">
-        <v>131</v>
-      </c>
+      <c r="F74" s="2"/>
       <c r="I74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4883,7 +4901,7 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -4900,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I76">
         <v>1</v>
@@ -4917,7 +4935,7 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I77">
         <v>1</v>
@@ -4934,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="I78">
         <v>1</v>
@@ -4951,7 +4969,7 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="I79">
         <v>1</v>
@@ -4968,7 +4986,7 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="I80">
         <v>1</v>
@@ -4985,7 +5003,7 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I81">
         <v>1</v>
@@ -5002,7 +5020,7 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I82">
         <v>1</v>
@@ -5013,16 +5031,16 @@
         <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>175</v>
-      </c>
-      <c r="C83" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>87</v>
       </c>
       <c r="I83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -5030,73 +5048,68 @@
         <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>64</v>
-      </c>
-      <c r="C84" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="F84" t="s">
-        <v>185</v>
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>88</v>
       </c>
       <c r="I84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>175</v>
-      </c>
-      <c r="C85" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
-      <c r="F85" s="2"/>
+      <c r="E85" t="s">
+        <v>89</v>
+      </c>
       <c r="I85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C86" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D86">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="I86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C87" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D87">
-        <v>1</v>
-      </c>
-      <c r="F87" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F87" t="s">
+        <v>184</v>
+      </c>
       <c r="I87">
         <v>0</v>
       </c>
@@ -5106,16 +5119,17 @@
         <v>164</v>
       </c>
       <c r="B88" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C88" t="s">
+        <v>177</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
-      <c r="E88" t="s">
-        <v>90</v>
-      </c>
+      <c r="F88" s="2"/>
       <c r="I88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -5123,13 +5137,16 @@
         <v>164</v>
       </c>
       <c r="B89" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C89" t="s">
+        <v>16</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
-      <c r="E89" t="s">
-        <v>135</v>
+      <c r="F89" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="I89">
         <v>1</v>
@@ -5140,16 +5157,17 @@
         <v>164</v>
       </c>
       <c r="B90" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C90" t="s">
+        <v>176</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
-      <c r="E90" t="s">
-        <v>136</v>
-      </c>
+      <c r="F90" s="2"/>
       <c r="I90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -5163,7 +5181,7 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="I91">
         <v>1</v>
@@ -5180,7 +5198,7 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I92">
         <v>1</v>
@@ -5197,7 +5215,7 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I93">
         <v>1</v>
@@ -5214,7 +5232,7 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="I94">
         <v>1</v>
@@ -5231,7 +5249,7 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="I95">
         <v>1</v>
@@ -5248,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="I96">
         <v>1</v>
@@ -5265,7 +5283,7 @@
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I97">
         <v>1</v>
@@ -5282,7 +5300,7 @@
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I98">
         <v>1</v>
@@ -5293,16 +5311,16 @@
         <v>164</v>
       </c>
       <c r="B99" t="s">
-        <v>175</v>
-      </c>
-      <c r="C99" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E99" t="s">
+        <v>93</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -5310,73 +5328,68 @@
         <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>64</v>
-      </c>
-      <c r="C100" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D100">
-        <v>0</v>
-      </c>
-      <c r="F100" t="s">
-        <v>186</v>
+        <v>1</v>
+      </c>
+      <c r="E100" t="s">
+        <v>94</v>
       </c>
       <c r="I100">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B101" t="s">
-        <v>175</v>
-      </c>
-      <c r="C101" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D101">
         <v>1</v>
       </c>
-      <c r="F101" s="2"/>
+      <c r="E101" t="s">
+        <v>95</v>
+      </c>
       <c r="I101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B102" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D102">
-        <v>1</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="I102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B103" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C103" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D103">
-        <v>1</v>
-      </c>
-      <c r="F103" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>185</v>
+      </c>
       <c r="I103">
         <v>0</v>
       </c>
@@ -5386,16 +5399,17 @@
         <v>165</v>
       </c>
       <c r="B104" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C104" t="s">
+        <v>177</v>
       </c>
       <c r="D104">
         <v>1</v>
       </c>
-      <c r="E104" t="s">
-        <v>96</v>
-      </c>
+      <c r="F104" s="2"/>
       <c r="I104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -5403,13 +5417,16 @@
         <v>165</v>
       </c>
       <c r="B105" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C105" t="s">
+        <v>16</v>
       </c>
       <c r="D105">
         <v>1</v>
       </c>
-      <c r="E105" t="s">
-        <v>140</v>
+      <c r="F105" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="I105">
         <v>1</v>
@@ -5420,16 +5437,17 @@
         <v>165</v>
       </c>
       <c r="B106" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C106" t="s">
+        <v>176</v>
       </c>
       <c r="D106">
         <v>1</v>
       </c>
-      <c r="E106" t="s">
-        <v>141</v>
-      </c>
+      <c r="F106" s="2"/>
       <c r="I106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -5443,7 +5461,7 @@
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="I107">
         <v>1</v>
@@ -5460,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I108">
         <v>1</v>
@@ -5477,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I109">
         <v>1</v>
@@ -5494,7 +5512,7 @@
         <v>1</v>
       </c>
       <c r="E110" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="I110">
         <v>1</v>
@@ -5511,7 +5529,7 @@
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="I111">
         <v>1</v>
@@ -5528,7 +5546,7 @@
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="I112">
         <v>1</v>
@@ -5545,7 +5563,7 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I113">
         <v>1</v>
@@ -5562,7 +5580,7 @@
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I114">
         <v>1</v>
@@ -5573,16 +5591,16 @@
         <v>165</v>
       </c>
       <c r="B115" t="s">
-        <v>175</v>
-      </c>
-      <c r="C115" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E115" t="s">
+        <v>117</v>
       </c>
       <c r="I115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -5590,73 +5608,68 @@
         <v>165</v>
       </c>
       <c r="B116" t="s">
-        <v>64</v>
-      </c>
-      <c r="C116" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D116">
-        <v>0</v>
-      </c>
-      <c r="F116" t="s">
-        <v>187</v>
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>118</v>
       </c>
       <c r="I116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B117" t="s">
-        <v>175</v>
-      </c>
-      <c r="C117" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D117">
         <v>1</v>
       </c>
-      <c r="F117" s="2"/>
+      <c r="E117" t="s">
+        <v>119</v>
+      </c>
       <c r="I117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B118" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C118" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D118">
-        <v>1</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="I118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B119" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C119" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D119">
-        <v>1</v>
-      </c>
-      <c r="F119" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F119" t="s">
+        <v>186</v>
+      </c>
       <c r="I119">
         <v>0</v>
       </c>
@@ -5666,16 +5679,17 @@
         <v>166</v>
       </c>
       <c r="B120" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C120" t="s">
+        <v>177</v>
       </c>
       <c r="D120">
         <v>1</v>
       </c>
-      <c r="E120" t="s">
-        <v>97</v>
-      </c>
+      <c r="F120" s="2"/>
       <c r="I120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5683,13 +5697,16 @@
         <v>166</v>
       </c>
       <c r="B121" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C121" t="s">
+        <v>16</v>
       </c>
       <c r="D121">
         <v>1</v>
       </c>
-      <c r="E121" t="s">
-        <v>145</v>
+      <c r="F121" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="I121">
         <v>1</v>
@@ -5700,16 +5717,17 @@
         <v>166</v>
       </c>
       <c r="B122" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C122" t="s">
+        <v>176</v>
       </c>
       <c r="D122">
         <v>1</v>
       </c>
-      <c r="E122" t="s">
-        <v>146</v>
-      </c>
+      <c r="F122" s="2"/>
       <c r="I122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -5723,7 +5741,7 @@
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="I123">
         <v>1</v>
@@ -5740,7 +5758,7 @@
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I124">
         <v>1</v>
@@ -5757,7 +5775,7 @@
         <v>1</v>
       </c>
       <c r="E125" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I125">
         <v>1</v>
@@ -5774,7 +5792,7 @@
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="I126">
         <v>1</v>
@@ -5791,7 +5809,7 @@
         <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="I127">
         <v>1</v>
@@ -5808,7 +5826,7 @@
         <v>1</v>
       </c>
       <c r="E128" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="I128">
         <v>1</v>
@@ -5825,7 +5843,7 @@
         <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I129">
         <v>1</v>
@@ -5842,7 +5860,7 @@
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I130">
         <v>1</v>
@@ -5853,16 +5871,16 @@
         <v>166</v>
       </c>
       <c r="B131" t="s">
-        <v>175</v>
-      </c>
-      <c r="C131" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E131" t="s">
+        <v>100</v>
       </c>
       <c r="I131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -5870,73 +5888,68 @@
         <v>166</v>
       </c>
       <c r="B132" t="s">
-        <v>64</v>
-      </c>
-      <c r="C132" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D132">
-        <v>0</v>
-      </c>
-      <c r="F132" t="s">
-        <v>188</v>
+        <v>1</v>
+      </c>
+      <c r="E132" t="s">
+        <v>101</v>
       </c>
       <c r="I132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B133" t="s">
-        <v>175</v>
-      </c>
-      <c r="C133" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D133">
         <v>1</v>
       </c>
-      <c r="F133" s="2"/>
+      <c r="E133" t="s">
+        <v>102</v>
+      </c>
       <c r="I133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B134" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C134" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D134">
-        <v>1</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="I134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B135" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C135" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D135">
-        <v>1</v>
-      </c>
-      <c r="F135" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F135" t="s">
+        <v>187</v>
+      </c>
       <c r="I135">
         <v>0</v>
       </c>
@@ -5946,16 +5959,17 @@
         <v>167</v>
       </c>
       <c r="B136" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C136" t="s">
+        <v>177</v>
       </c>
       <c r="D136">
         <v>1</v>
       </c>
-      <c r="E136" t="s">
-        <v>103</v>
-      </c>
+      <c r="F136" s="2"/>
       <c r="I136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5963,13 +5977,16 @@
         <v>167</v>
       </c>
       <c r="B137" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C137" t="s">
+        <v>16</v>
       </c>
       <c r="D137">
         <v>1</v>
       </c>
-      <c r="E137" t="s">
-        <v>150</v>
+      <c r="F137" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="I137">
         <v>1</v>
@@ -5980,16 +5997,17 @@
         <v>167</v>
       </c>
       <c r="B138" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C138" t="s">
+        <v>176</v>
       </c>
       <c r="D138">
         <v>1</v>
       </c>
-      <c r="E138" t="s">
-        <v>151</v>
-      </c>
+      <c r="F138" s="2"/>
       <c r="I138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -6003,7 +6021,7 @@
         <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="I139">
         <v>1</v>
@@ -6020,7 +6038,7 @@
         <v>1</v>
       </c>
       <c r="E140" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I140">
         <v>1</v>
@@ -6037,7 +6055,7 @@
         <v>1</v>
       </c>
       <c r="E141" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I141">
         <v>1</v>
@@ -6054,7 +6072,7 @@
         <v>1</v>
       </c>
       <c r="E142" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="I142">
         <v>1</v>
@@ -6071,7 +6089,7 @@
         <v>1</v>
       </c>
       <c r="E143" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="I143">
         <v>1</v>
@@ -6088,7 +6106,7 @@
         <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="I144">
         <v>1</v>
@@ -6105,7 +6123,7 @@
         <v>1</v>
       </c>
       <c r="E145" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I145">
         <v>1</v>
@@ -6122,7 +6140,7 @@
         <v>1</v>
       </c>
       <c r="E146" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I146">
         <v>1</v>
@@ -6133,16 +6151,16 @@
         <v>167</v>
       </c>
       <c r="B147" t="s">
-        <v>175</v>
-      </c>
-      <c r="C147" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E147" t="s">
+        <v>106</v>
       </c>
       <c r="I147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -6150,73 +6168,68 @@
         <v>167</v>
       </c>
       <c r="B148" t="s">
-        <v>64</v>
-      </c>
-      <c r="C148" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="D148">
-        <v>0</v>
-      </c>
-      <c r="F148" t="s">
-        <v>189</v>
+        <v>1</v>
+      </c>
+      <c r="E148" t="s">
+        <v>107</v>
       </c>
       <c r="I148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B149" t="s">
-        <v>175</v>
-      </c>
-      <c r="C149" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D149">
         <v>1</v>
       </c>
-      <c r="F149" s="2"/>
+      <c r="E149" t="s">
+        <v>108</v>
+      </c>
       <c r="I149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B150" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="C150" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="D150">
-        <v>1</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="I150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B151" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="C151" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D151">
-        <v>1</v>
-      </c>
-      <c r="F151" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F151" t="s">
+        <v>188</v>
+      </c>
       <c r="I151">
         <v>0</v>
       </c>
@@ -6226,16 +6239,17 @@
         <v>168</v>
       </c>
       <c r="B152" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C152" t="s">
+        <v>177</v>
       </c>
       <c r="D152">
         <v>1</v>
       </c>
-      <c r="E152" t="s">
-        <v>109</v>
-      </c>
+      <c r="F152" s="2"/>
       <c r="I152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -6243,13 +6257,16 @@
         <v>168</v>
       </c>
       <c r="B153" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C153" t="s">
+        <v>16</v>
       </c>
       <c r="D153">
         <v>1</v>
       </c>
-      <c r="E153" t="s">
-        <v>155</v>
+      <c r="F153" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="I153">
         <v>1</v>
@@ -6260,16 +6277,17 @@
         <v>168</v>
       </c>
       <c r="B154" t="s">
-        <v>62</v>
+        <v>174</v>
+      </c>
+      <c r="C154" t="s">
+        <v>176</v>
       </c>
       <c r="D154">
         <v>1</v>
       </c>
-      <c r="E154" t="s">
-        <v>156</v>
-      </c>
+      <c r="F154" s="2"/>
       <c r="I154">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -6283,7 +6301,7 @@
         <v>1</v>
       </c>
       <c r="E155" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="I155">
         <v>1</v>
@@ -6300,7 +6318,7 @@
         <v>1</v>
       </c>
       <c r="E156" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I156">
         <v>1</v>
@@ -6317,7 +6335,7 @@
         <v>1</v>
       </c>
       <c r="E157" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I157">
         <v>1</v>
@@ -6334,7 +6352,7 @@
         <v>1</v>
       </c>
       <c r="E158" t="s">
-        <v>110</v>
+        <v>157</v>
       </c>
       <c r="I158">
         <v>1</v>
@@ -6351,7 +6369,7 @@
         <v>1</v>
       </c>
       <c r="E159" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="I159">
         <v>1</v>
@@ -6368,7 +6386,7 @@
         <v>1</v>
       </c>
       <c r="E160" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
       <c r="I160">
         <v>1</v>
@@ -6385,7 +6403,7 @@
         <v>1</v>
       </c>
       <c r="E161" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I161">
         <v>1</v>
@@ -6402,7 +6420,7 @@
         <v>1</v>
       </c>
       <c r="E162" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I162">
         <v>1</v>
@@ -6413,16 +6431,16 @@
         <v>168</v>
       </c>
       <c r="B163" t="s">
-        <v>175</v>
-      </c>
-      <c r="C163" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E163" t="s">
+        <v>112</v>
       </c>
       <c r="I163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -6430,18 +6448,69 @@
         <v>168</v>
       </c>
       <c r="B164" t="s">
+        <v>62</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164" t="s">
+        <v>113</v>
+      </c>
+      <c r="I164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>168</v>
+      </c>
+      <c r="B165" t="s">
+        <v>62</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165" t="s">
+        <v>114</v>
+      </c>
+      <c r="I165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>168</v>
+      </c>
+      <c r="B166" t="s">
+        <v>174</v>
+      </c>
+      <c r="C166" t="s">
+        <v>175</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="I166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>168</v>
+      </c>
+      <c r="B167" t="s">
         <v>64</v>
       </c>
-      <c r="C164" t="s">
-        <v>172</v>
-      </c>
-      <c r="D164">
-        <v>0</v>
-      </c>
-      <c r="F164" t="s">
-        <v>190</v>
-      </c>
-      <c r="I164">
+      <c r="C167" t="s">
+        <v>171</v>
+      </c>
+      <c r="D167">
+        <v>0</v>
+      </c>
+      <c r="F167" t="s">
+        <v>189</v>
+      </c>
+      <c r="I167">
         <v>0</v>
       </c>
     </row>
@@ -6454,16 +6523,16 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{525B56D9-62C4-48D6-967A-354412BC18DC}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{C154652A-BDF9-4615-B1E4-499FEF1EDC11}"/>
-    <hyperlink ref="F22" r:id="rId3" xr:uid="{30629169-7EA1-4243-84C3-FA4D064C9822}"/>
-    <hyperlink ref="F38" r:id="rId4" xr:uid="{AC7E6380-3928-4471-8B34-653513FE324C}"/>
-    <hyperlink ref="F54" r:id="rId5" xr:uid="{831A21C6-C66A-476B-9807-15FFCF98A76C}"/>
-    <hyperlink ref="F70" r:id="rId6" xr:uid="{491AE70B-7299-4601-BE3E-79603CE0F309}"/>
-    <hyperlink ref="F102" r:id="rId7" xr:uid="{41ECC269-CF81-4F58-9AF2-FDDD27815200}"/>
-    <hyperlink ref="F118" r:id="rId8" xr:uid="{D2C4EA41-24BE-43B2-90C6-EE10B5800DA2}"/>
-    <hyperlink ref="F134" r:id="rId9" xr:uid="{BBC1F586-A111-4249-9776-C2B3698C39CB}"/>
-    <hyperlink ref="F150" r:id="rId10" xr:uid="{6A654793-5A62-49E1-929A-410DB9EC0DD3}"/>
-    <hyperlink ref="F86" r:id="rId11" xr:uid="{1512ACF6-D2A6-4364-81B1-D816FFF32408}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{C154652A-BDF9-4615-B1E4-499FEF1EDC11}"/>
+    <hyperlink ref="F25" r:id="rId3" xr:uid="{30629169-7EA1-4243-84C3-FA4D064C9822}"/>
+    <hyperlink ref="F41" r:id="rId4" xr:uid="{AC7E6380-3928-4471-8B34-653513FE324C}"/>
+    <hyperlink ref="F57" r:id="rId5" xr:uid="{831A21C6-C66A-476B-9807-15FFCF98A76C}"/>
+    <hyperlink ref="F73" r:id="rId6" xr:uid="{491AE70B-7299-4601-BE3E-79603CE0F309}"/>
+    <hyperlink ref="F105" r:id="rId7" xr:uid="{41ECC269-CF81-4F58-9AF2-FDDD27815200}"/>
+    <hyperlink ref="F121" r:id="rId8" xr:uid="{D2C4EA41-24BE-43B2-90C6-EE10B5800DA2}"/>
+    <hyperlink ref="F137" r:id="rId9" xr:uid="{BBC1F586-A111-4249-9776-C2B3698C39CB}"/>
+    <hyperlink ref="F153" r:id="rId10" xr:uid="{6A654793-5A62-49E1-929A-410DB9EC0DD3}"/>
+    <hyperlink ref="F89" r:id="rId11" xr:uid="{1512ACF6-D2A6-4364-81B1-D816FFF32408}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>

</xml_diff>